<commit_message>
Processed Results - nexus 5x until microphone
</commit_message>
<xml_diff>
--- a/Processed Results/Nexus 5X/Local Storage/Local Storage - Processed.xlsx
+++ b/Processed Results/Nexus 5X/Local Storage/Local Storage - Processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Nexus 5X\Local Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6411E38-0456-4426-84B3-EDB08C1C21F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AA595F-55E4-4DA2-857E-7561A2372B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
+    <workbookView xWindow="130" yWindow="120" windowWidth="9990" windowHeight="9830" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Blad1!$A$98:$A$187</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Blad1!$B$98:$B$187</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$66:$A$95</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$65</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$B$66:$B$95</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$A$34:$A$63</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$33</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$B$34:$B$63</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$A$98:$A$187</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$98:$B$187</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$34:$A$63</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$33</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$B$34:$B$63</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$A$98:$A$187</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$98:$B$187</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$A$66:$A$95</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$B$65</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$66:$B$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -285,94 +285,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>111.838104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.518491999999995</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.723072000000002</c:v>
+                  <c:v>126.405252</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.882155999999995</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.927651999999995</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.086735999999902</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96.404904000000002</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95.768567999999902</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97.359408000000002</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96.404904000000002</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>124.682256</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95.927651999999995</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.723072000000002</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96.404904000000002</c:v>
+                  <c:v>126.561888</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>95.291315999999995</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>95.609483999999995</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>95.927651999999995</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96.086735999999902</c:v>
+                  <c:v>126.561888</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>96.563987999999995</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>96.723072000000002</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>96.563987999999995</c:v>
+                  <c:v>117.633636</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>95.927651999999995</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96.086735999999902</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>95.927651999999995</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>96.404904000000002</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>96.404904000000002</c:v>
+                  <c:v>125.778707999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>96.245819999999995</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,10 +456,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>96.304150799999974</c:v>
+                  <c:v>126.12330719999981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.304150799999974</c:v>
+                  <c:v>126.12330719999981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,94 +920,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>96.547499999999999</c:v>
+                  <c:v>112.93455599999901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.492500000000007</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.334999999999994</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.075000000000003</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.862499999999997</c:v>
+                  <c:v>127.814976</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.704999999999998</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97.02</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>97.334999999999994</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.177499999999995</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95.759999999999906</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96.547499999999999</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95.917500000000004</c:v>
+                  <c:v>125.465436</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>97.02</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.965000000000003</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97.02</c:v>
+                  <c:v>126.248616</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>96.075000000000003</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96.862499999999997</c:v>
+                  <c:v>126.561888</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>96.075000000000003</c:v>
+                  <c:v>126.87515999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>96.547499999999999</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96.704999999999998</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>98.4375</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>97.02</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>98.4375</c:v>
+                  <c:v>123.89907599999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>97.02</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96.862499999999997</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>96.075000000000003</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>95.444999999999993</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>95.917500000000004</c:v>
+                  <c:v>126.71852399999899</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>96.232500000000002</c:v>
+                  <c:v>126.09198000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>97.177499999999995</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,10 +1059,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>96.788999999999987</c:v>
+                  <c:v>126.42613679999967</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.788999999999987</c:v>
+                  <c:v>126.42613679999967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,7 +1206,6 @@
         <c:axId val="489458320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="98.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1615,94 +1614,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>162.90144000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.701183999999998</c:v>
+                  <c:v>129.22469999999899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.383087999999901</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.701183999999998</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.269751999999997</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>128.12824800000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>96.224039999999903</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>123.585804</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96.224039999999903</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.383087999999901</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>127.97161199999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>97.019279999999995</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>96.701183999999998</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>98.132615999999999</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96.224039999999903</c:v>
+                  <c:v>127.031796</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>96.542135999999999</c:v>
+                  <c:v>127.65834</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>97.973568</c:v>
+                  <c:v>128.28488399999901</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>96.860231999999996</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96.064992000000004</c:v>
+                  <c:v>127.501704</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>96.383087999999901</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>96.224039999999903</c:v>
+                  <c:v>127.97161199999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>96.383087999999901</c:v>
+                  <c:v>127.345068</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>97.178327999999993</c:v>
+                  <c:v>124.838892</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>95.746895999999893</c:v>
+                  <c:v>127.188431999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,10 +1753,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>96.478516799999994</c:v>
+                  <c:v>128.57204999999982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.478516799999994</c:v>
+                  <c:v>128.57204999999982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,7 +1900,8 @@
         <c:axId val="281410968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="95"/>
+          <c:max val="165"/>
+          <c:min val="120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2182,7 +2182,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="98" min="95"/>
+        <cx:valScaling min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2225,10 +2225,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2303,7 +2303,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling min="95"/>
+        <cx:valScaling max="165" min="110"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2346,10 +2346,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2387,7 +2387,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3F5A16A3-6E4C-4475-A634-1322A70DC713}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Medium_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2431,7 +2431,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="98.5" min="95"/>
+        <cx:valScaling min="112"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2474,10 +2474,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2515,7 +2515,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{138ACD3C-CAEA-4AEF-B3DF-B982F1EA92CC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>High_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2559,7 +2559,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="98.5" min="95"/>
+        <cx:valScaling max="165" min="120"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -7209,8 +7209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FE0459-F6C0-45BE-AD60-56F63431C3F0}">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U98" sqref="U98"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B99" activeCellId="1" sqref="B98 B99:B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7233,7 +7233,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>96.245819999999995</v>
+        <v>111.838104</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
@@ -7247,14 +7247,14 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>97.518491999999995</v>
+        <v>127.65834</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>96.304150799999974</v>
+        <v>126.12330719999981</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -7262,14 +7262,14 @@
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>96.723072000000002</v>
+        <v>126.405252</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>96.304150799999974</v>
+        <v>126.12330719999981</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -7277,7 +7277,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>96.882155999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -7285,7 +7285,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>96.245819999999995</v>
+        <v>127.501704</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -7299,15 +7299,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>95.927651999999995</v>
+        <v>126.87515999999999</v>
       </c>
       <c r="D7" s="1">
         <f>MIN(B2:B31)</f>
-        <v>95.291315999999995</v>
+        <v>111.838104</v>
       </c>
       <c r="E7" s="1">
         <f>MAX(B2:B31)</f>
-        <v>97.518491999999995</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -7315,7 +7315,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>96.086735999999902</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -7323,7 +7323,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>96.404904000000002</v>
+        <v>127.188431999999</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -7337,15 +7337,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>95.768567999999902</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="D10">
         <f>QUARTILE(B2:B31, 1)</f>
-        <v>95.967422999999968</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="E10">
         <f>QUARTILE(B2:B31, 2)</f>
-        <v>96.245819999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -7353,7 +7353,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>97.359408000000002</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -7361,7 +7361,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>96.404904000000002</v>
+        <v>127.031796</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -7375,15 +7375,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>96.245819999999995</v>
+        <v>124.682256</v>
       </c>
       <c r="D13">
         <f>QUARTILE(B2:B31, 3)</f>
-        <v>96.524216999999993</v>
+        <v>127.345068</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> D13 - D10</f>
-        <v>0.55679400000002488</v>
+        <v>0.62654400000100452</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -7391,7 +7391,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>95.927651999999995</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -7399,7 +7399,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>96.723072000000002</v>
+        <v>127.345068</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -7413,15 +7413,15 @@
         <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>96.404904000000002</v>
+        <v>126.561888</v>
       </c>
       <c r="D16">
         <f>STDEV(B2:B31)</f>
-        <v>0.46612039492215035</v>
+        <v>3.2400930122428142</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (D16 / E4) * 100</f>
-        <v>0.48400862377174969</v>
+        <v>2.5689883053136584</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -7429,7 +7429,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>95.291315999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -7437,7 +7437,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1">
-        <v>95.609483999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -7445,7 +7445,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="1">
-        <v>95.927651999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7453,7 +7453,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>96.245819999999995</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -7461,7 +7461,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="1">
-        <v>96.086735999999902</v>
+        <v>126.561888</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -7469,7 +7469,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1">
-        <v>96.563987999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -7477,7 +7477,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="1">
-        <v>96.723072000000002</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -7485,7 +7485,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1">
-        <v>96.563987999999995</v>
+        <v>117.633636</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -7493,7 +7493,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>95.927651999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -7501,7 +7501,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="1">
-        <v>96.086735999999902</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -7509,7 +7509,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1">
-        <v>95.927651999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -7517,7 +7517,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="1">
-        <v>96.245819999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -7525,7 +7525,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="1">
-        <v>96.404904000000002</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -7533,7 +7533,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1">
-        <v>96.404904000000002</v>
+        <v>125.778707999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -7541,7 +7541,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="1">
-        <v>96.245819999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -7560,7 +7560,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="1">
-        <v>96.547499999999999</v>
+        <v>112.93455599999901</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -7574,14 +7574,14 @@
         <v>12</v>
       </c>
       <c r="B35" s="1">
-        <v>97.492500000000007</v>
+        <v>127.65834</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>96.788999999999987</v>
+        <v>126.42613679999967</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -7589,14 +7589,14 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <v>97.334999999999994</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="D36">
         <v>30</v>
       </c>
       <c r="E36" s="1">
         <f>AVERAGE(B34,B35,B36,B37,B38,B39,B40,B41,B42,B43,B44,B45,B46,B47,B48,B49,B50,B51,B53,B52,B54,B55,B56,B57,B58,B59,B60,B61,B62,B63)</f>
-        <v>96.788999999999987</v>
+        <v>126.42613679999967</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -7604,7 +7604,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="1">
-        <v>96.075000000000003</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -7612,7 +7612,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="1">
-        <v>96.862499999999997</v>
+        <v>127.814976</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>3</v>
@@ -7626,15 +7626,15 @@
         <v>12</v>
       </c>
       <c r="B39" s="1">
-        <v>96.704999999999998</v>
+        <v>127.188431999999</v>
       </c>
       <c r="D39" s="1">
         <f>MIN(B34:B63)</f>
-        <v>95.444999999999993</v>
+        <v>112.93455599999901</v>
       </c>
       <c r="E39" s="1">
         <f>MAX(B34:B63)</f>
-        <v>98.4375</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -7642,7 +7642,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="1">
-        <v>97.02</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -7650,7 +7650,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="1">
-        <v>97.334999999999994</v>
+        <v>127.031796</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
@@ -7664,15 +7664,15 @@
         <v>12</v>
       </c>
       <c r="B42" s="1">
-        <v>97.177499999999995</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="D42">
         <f>QUARTILE(B34:B63, 1)</f>
-        <v>96.114374999999995</v>
+        <v>126.71852399999899</v>
       </c>
       <c r="E42">
         <f>QUARTILE(B34:B63, 2)</f>
-        <v>96.862499999999997</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -7680,7 +7680,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="1">
-        <v>95.759999999999906</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -7688,7 +7688,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="1">
-        <v>96.547499999999999</v>
+        <v>127.031796</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
@@ -7702,15 +7702,15 @@
         <v>12</v>
       </c>
       <c r="B45" s="1">
-        <v>95.917500000000004</v>
+        <v>125.465436</v>
       </c>
       <c r="D45">
         <f>QUARTILE(B34:B63, 3)</f>
-        <v>97.138125000000002</v>
+        <v>127.188431999999</v>
       </c>
       <c r="E45">
         <f xml:space="preserve"> D45 - D42</f>
-        <v>1.0237500000000068</v>
+        <v>0.46990800000000377</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -7718,7 +7718,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="1">
-        <v>97.02</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -7726,7 +7726,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="1">
-        <v>97.965000000000003</v>
+        <v>127.031796</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>16</v>
@@ -7740,15 +7740,15 @@
         <v>12</v>
       </c>
       <c r="B48" s="1">
-        <v>97.02</v>
+        <v>126.248616</v>
       </c>
       <c r="D48">
         <f>STDEV(B34:B63)</f>
-        <v>0.72910567561012873</v>
+        <v>2.6616149853139786</v>
       </c>
       <c r="E48">
         <f xml:space="preserve"> (D48 / E36) * 100</f>
-        <v>0.75329394415701045</v>
+        <v>2.1052727329037437</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -7756,7 +7756,7 @@
         <v>12</v>
       </c>
       <c r="B49" s="1">
-        <v>96.075000000000003</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -7764,7 +7764,7 @@
         <v>12</v>
       </c>
       <c r="B50" s="1">
-        <v>96.862499999999997</v>
+        <v>126.561888</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -7772,7 +7772,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="1">
-        <v>96.075000000000003</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -7780,7 +7780,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="1">
-        <v>96.547499999999999</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -7788,7 +7788,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="1">
-        <v>96.704999999999998</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -7796,7 +7796,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="1">
-        <v>98.4375</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -7804,7 +7804,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="1">
-        <v>97.02</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -7812,7 +7812,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="1">
-        <v>98.4375</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -7820,7 +7820,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="1">
-        <v>97.02</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -7828,7 +7828,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1">
-        <v>96.862499999999997</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -7836,7 +7836,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="1">
-        <v>96.075000000000003</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -7844,7 +7844,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="1">
-        <v>95.444999999999993</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -7852,7 +7852,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="1">
-        <v>95.917500000000004</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -7860,7 +7860,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="1">
-        <v>96.232500000000002</v>
+        <v>126.09198000000001</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -7868,7 +7868,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="1">
-        <v>97.177499999999995</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -7887,7 +7887,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="1">
-        <v>96.542135999999999</v>
+        <v>162.90144000000001</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -7901,14 +7901,14 @@
         <v>14</v>
       </c>
       <c r="B67" s="1">
-        <v>96.701183999999998</v>
+        <v>129.22469999999899</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>96.478516799999994</v>
+        <v>128.57204999999982</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -7916,14 +7916,14 @@
         <v>14</v>
       </c>
       <c r="B68" s="1">
-        <v>96.542135999999999</v>
+        <v>127.345068</v>
       </c>
       <c r="D68">
         <v>30</v>
       </c>
       <c r="E68" s="1">
         <f>AVERAGE(B66,B67,B68,B69,B70,B71,B72,B73,B74,B75,B76,B77,B78,B79,B80,B81,B82,B83,B85,B84,B86,B87,B88,B89,B90,B91,B92,B93,B94,B95)</f>
-        <v>96.478516799999994</v>
+        <v>128.57204999999982</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -7931,7 +7931,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="1">
-        <v>96.383087999999901</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -7939,7 +7939,7 @@
         <v>14</v>
       </c>
       <c r="B70" s="1">
-        <v>96.701183999999998</v>
+        <v>128.12824800000001</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>3</v>
@@ -7953,15 +7953,15 @@
         <v>14</v>
       </c>
       <c r="B71" s="1">
-        <v>95.269751999999997</v>
+        <v>127.501704</v>
       </c>
       <c r="D71" s="1">
         <f>MIN(B66:B95)</f>
-        <v>95.269751999999997</v>
+        <v>123.585804</v>
       </c>
       <c r="E71" s="1">
         <f>MAX(B66:B95)</f>
-        <v>98.132615999999999</v>
+        <v>162.90144000000001</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -7969,7 +7969,7 @@
         <v>14</v>
       </c>
       <c r="B72" s="1">
-        <v>96.542135999999999</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -7977,7 +7977,7 @@
         <v>14</v>
       </c>
       <c r="B73" s="1">
-        <v>96.064992000000004</v>
+        <v>128.12824800000001</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>5</v>
@@ -7991,15 +7991,15 @@
         <v>14</v>
       </c>
       <c r="B74" s="1">
-        <v>96.064992000000004</v>
+        <v>127.031796</v>
       </c>
       <c r="D74">
         <f>QUARTILE(B66:B95, 1)</f>
-        <v>96.104753999999986</v>
+        <v>127.22759099999925</v>
       </c>
       <c r="E74">
         <f>QUARTILE(B66:B95, 2)</f>
-        <v>96.383087999999901</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -8007,7 +8007,7 @@
         <v>14</v>
       </c>
       <c r="B75" s="1">
-        <v>96.224039999999903</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -8015,7 +8015,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="1">
-        <v>96.542135999999999</v>
+        <v>127.188431999999</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
@@ -8029,15 +8029,15 @@
         <v>14</v>
       </c>
       <c r="B77" s="1">
-        <v>96.542135999999999</v>
+        <v>123.585804</v>
       </c>
       <c r="D77">
         <f>QUARTILE(B66:B95, 3)</f>
-        <v>96.661422000000002</v>
+        <v>127.97161199999999</v>
       </c>
       <c r="E77">
         <f xml:space="preserve"> D77 - D74</f>
-        <v>0.55666800000001615</v>
+        <v>0.74402100000074256</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -8045,7 +8045,7 @@
         <v>14</v>
       </c>
       <c r="B78" s="1">
-        <v>96.224039999999903</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -8053,7 +8053,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="1">
-        <v>96.383087999999901</v>
+        <v>127.65834</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>16</v>
@@ -8067,15 +8067,15 @@
         <v>14</v>
       </c>
       <c r="B80" s="1">
-        <v>96.064992000000004</v>
+        <v>127.345068</v>
       </c>
       <c r="D80">
         <f>STDEV(B66:B95)</f>
-        <v>0.56902742349663038</v>
+        <v>6.5596621899091456</v>
       </c>
       <c r="E80">
         <f xml:space="preserve"> (D80 / E68) * 100</f>
-        <v>0.58979702670618839</v>
+        <v>5.1019348216888156</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -8083,7 +8083,7 @@
         <v>14</v>
       </c>
       <c r="B81" s="1">
-        <v>96.064992000000004</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -8091,7 +8091,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="1">
-        <v>97.019279999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -8099,7 +8099,7 @@
         <v>14</v>
       </c>
       <c r="B83" s="1">
-        <v>96.701183999999998</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -8107,7 +8107,7 @@
         <v>14</v>
       </c>
       <c r="B84" s="1">
-        <v>98.132615999999999</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -8115,7 +8115,7 @@
         <v>14</v>
       </c>
       <c r="B85" s="1">
-        <v>96.224039999999903</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -8123,7 +8123,7 @@
         <v>14</v>
       </c>
       <c r="B86" s="1">
-        <v>96.064992000000004</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -8131,7 +8131,7 @@
         <v>14</v>
       </c>
       <c r="B87" s="1">
-        <v>96.542135999999999</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -8139,7 +8139,7 @@
         <v>14</v>
       </c>
       <c r="B88" s="1">
-        <v>97.973568</v>
+        <v>128.28488399999901</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -8147,7 +8147,7 @@
         <v>14</v>
       </c>
       <c r="B89" s="1">
-        <v>96.860231999999996</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -8155,7 +8155,7 @@
         <v>14</v>
       </c>
       <c r="B90" s="1">
-        <v>96.064992000000004</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -8163,7 +8163,7 @@
         <v>14</v>
       </c>
       <c r="B91" s="1">
-        <v>96.383087999999901</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -8171,7 +8171,7 @@
         <v>14</v>
       </c>
       <c r="B92" s="1">
-        <v>96.224039999999903</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -8179,7 +8179,7 @@
         <v>14</v>
       </c>
       <c r="B93" s="1">
-        <v>96.383087999999901</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -8187,7 +8187,7 @@
         <v>14</v>
       </c>
       <c r="B94" s="1">
-        <v>97.178327999999993</v>
+        <v>124.838892</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -8195,7 +8195,7 @@
         <v>14</v>
       </c>
       <c r="B95" s="1">
-        <v>95.746895999999893</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -8211,7 +8211,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="1">
-        <v>96.245819999999995</v>
+        <v>111.838104</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -8219,7 +8219,7 @@
         <v>10</v>
       </c>
       <c r="B99" s="1">
-        <v>97.518491999999995</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -8227,7 +8227,7 @@
         <v>10</v>
       </c>
       <c r="B100" s="1">
-        <v>96.723072000000002</v>
+        <v>126.405252</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -8235,7 +8235,7 @@
         <v>10</v>
       </c>
       <c r="B101" s="1">
-        <v>96.882155999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -8243,7 +8243,7 @@
         <v>10</v>
       </c>
       <c r="B102" s="1">
-        <v>96.245819999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -8251,7 +8251,7 @@
         <v>10</v>
       </c>
       <c r="B103" s="1">
-        <v>95.927651999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -8259,7 +8259,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="1">
-        <v>96.086735999999902</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -8267,7 +8267,7 @@
         <v>10</v>
       </c>
       <c r="B105" s="1">
-        <v>96.404904000000002</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -8275,7 +8275,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="1">
-        <v>95.768567999999902</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -8283,7 +8283,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="1">
-        <v>97.359408000000002</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -8291,7 +8291,7 @@
         <v>10</v>
       </c>
       <c r="B108" s="1">
-        <v>96.404904000000002</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -8299,7 +8299,7 @@
         <v>10</v>
       </c>
       <c r="B109" s="1">
-        <v>96.245819999999995</v>
+        <v>124.682256</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -8307,7 +8307,7 @@
         <v>10</v>
       </c>
       <c r="B110" s="1">
-        <v>95.927651999999995</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -8315,7 +8315,7 @@
         <v>10</v>
       </c>
       <c r="B111" s="1">
-        <v>96.723072000000002</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -8323,7 +8323,7 @@
         <v>10</v>
       </c>
       <c r="B112" s="1">
-        <v>96.404904000000002</v>
+        <v>126.561888</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -8331,7 +8331,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="1">
-        <v>95.291315999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -8339,7 +8339,7 @@
         <v>10</v>
       </c>
       <c r="B114" s="1">
-        <v>95.609483999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -8347,7 +8347,7 @@
         <v>10</v>
       </c>
       <c r="B115" s="1">
-        <v>95.927651999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -8355,7 +8355,7 @@
         <v>10</v>
       </c>
       <c r="B116" s="1">
-        <v>96.245819999999995</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -8363,7 +8363,7 @@
         <v>10</v>
       </c>
       <c r="B117" s="1">
-        <v>96.086735999999902</v>
+        <v>126.561888</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -8371,7 +8371,7 @@
         <v>10</v>
       </c>
       <c r="B118" s="1">
-        <v>96.563987999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -8379,7 +8379,7 @@
         <v>10</v>
       </c>
       <c r="B119" s="1">
-        <v>96.723072000000002</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -8387,7 +8387,7 @@
         <v>10</v>
       </c>
       <c r="B120" s="1">
-        <v>96.563987999999995</v>
+        <v>117.633636</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -8395,7 +8395,7 @@
         <v>10</v>
       </c>
       <c r="B121" s="1">
-        <v>95.927651999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -8403,7 +8403,7 @@
         <v>10</v>
       </c>
       <c r="B122" s="1">
-        <v>96.086735999999902</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -8411,7 +8411,7 @@
         <v>10</v>
       </c>
       <c r="B123" s="1">
-        <v>95.927651999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -8419,7 +8419,7 @@
         <v>10</v>
       </c>
       <c r="B124" s="1">
-        <v>96.245819999999995</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -8427,7 +8427,7 @@
         <v>10</v>
       </c>
       <c r="B125" s="1">
-        <v>96.404904000000002</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -8435,7 +8435,7 @@
         <v>10</v>
       </c>
       <c r="B126" s="1">
-        <v>96.404904000000002</v>
+        <v>125.778707999999</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -8443,7 +8443,7 @@
         <v>10</v>
       </c>
       <c r="B127" s="1">
-        <v>96.245819999999995</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -8451,7 +8451,7 @@
         <v>12</v>
       </c>
       <c r="B128" s="1">
-        <v>96.547499999999999</v>
+        <v>112.93455599999901</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -8459,7 +8459,7 @@
         <v>12</v>
       </c>
       <c r="B129" s="1">
-        <v>97.492500000000007</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -8467,7 +8467,7 @@
         <v>12</v>
       </c>
       <c r="B130" s="1">
-        <v>97.334999999999994</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -8475,7 +8475,7 @@
         <v>12</v>
       </c>
       <c r="B131" s="1">
-        <v>96.075000000000003</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -8483,7 +8483,7 @@
         <v>12</v>
       </c>
       <c r="B132" s="1">
-        <v>96.862499999999997</v>
+        <v>127.814976</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -8491,7 +8491,7 @@
         <v>12</v>
       </c>
       <c r="B133" s="1">
-        <v>96.704999999999998</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -8499,7 +8499,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="1">
-        <v>97.02</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -8507,7 +8507,7 @@
         <v>12</v>
       </c>
       <c r="B135" s="1">
-        <v>97.334999999999994</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -8515,7 +8515,7 @@
         <v>12</v>
       </c>
       <c r="B136" s="1">
-        <v>97.177499999999995</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -8523,7 +8523,7 @@
         <v>12</v>
       </c>
       <c r="B137" s="1">
-        <v>95.759999999999906</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -8531,7 +8531,7 @@
         <v>12</v>
       </c>
       <c r="B138" s="1">
-        <v>96.547499999999999</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -8539,7 +8539,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="1">
-        <v>95.917500000000004</v>
+        <v>125.465436</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -8547,7 +8547,7 @@
         <v>12</v>
       </c>
       <c r="B140" s="1">
-        <v>97.02</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -8555,7 +8555,7 @@
         <v>12</v>
       </c>
       <c r="B141" s="1">
-        <v>97.965000000000003</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -8563,7 +8563,7 @@
         <v>12</v>
       </c>
       <c r="B142" s="1">
-        <v>97.02</v>
+        <v>126.248616</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -8571,7 +8571,7 @@
         <v>12</v>
       </c>
       <c r="B143" s="1">
-        <v>96.075000000000003</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -8579,7 +8579,7 @@
         <v>12</v>
       </c>
       <c r="B144" s="1">
-        <v>96.862499999999997</v>
+        <v>126.561888</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -8587,7 +8587,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="1">
-        <v>96.075000000000003</v>
+        <v>126.87515999999999</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -8595,7 +8595,7 @@
         <v>12</v>
       </c>
       <c r="B146" s="1">
-        <v>96.547499999999999</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -8603,7 +8603,7 @@
         <v>12</v>
       </c>
       <c r="B147" s="1">
-        <v>96.704999999999998</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -8611,7 +8611,7 @@
         <v>12</v>
       </c>
       <c r="B148" s="1">
-        <v>98.4375</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -8619,7 +8619,7 @@
         <v>12</v>
       </c>
       <c r="B149" s="1">
-        <v>97.02</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -8627,7 +8627,7 @@
         <v>12</v>
       </c>
       <c r="B150" s="1">
-        <v>98.4375</v>
+        <v>123.89907599999999</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -8635,7 +8635,7 @@
         <v>12</v>
       </c>
       <c r="B151" s="1">
-        <v>97.02</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -8643,7 +8643,7 @@
         <v>12</v>
       </c>
       <c r="B152" s="1">
-        <v>96.862499999999997</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -8651,7 +8651,7 @@
         <v>12</v>
       </c>
       <c r="B153" s="1">
-        <v>96.075000000000003</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -8659,7 +8659,7 @@
         <v>12</v>
       </c>
       <c r="B154" s="1">
-        <v>95.444999999999993</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -8667,7 +8667,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="1">
-        <v>95.917500000000004</v>
+        <v>126.71852399999899</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -8675,7 +8675,7 @@
         <v>12</v>
       </c>
       <c r="B156" s="1">
-        <v>96.232500000000002</v>
+        <v>126.09198000000001</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -8683,7 +8683,7 @@
         <v>12</v>
       </c>
       <c r="B157" s="1">
-        <v>97.177499999999995</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -8691,7 +8691,7 @@
         <v>14</v>
       </c>
       <c r="B158" s="1">
-        <v>96.542135999999999</v>
+        <v>162.90144000000001</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -8699,7 +8699,7 @@
         <v>14</v>
       </c>
       <c r="B159" s="1">
-        <v>96.701183999999998</v>
+        <v>129.22469999999899</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -8707,7 +8707,7 @@
         <v>14</v>
       </c>
       <c r="B160" s="1">
-        <v>96.542135999999999</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -8715,7 +8715,7 @@
         <v>14</v>
       </c>
       <c r="B161" s="1">
-        <v>96.383087999999901</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -8723,7 +8723,7 @@
         <v>14</v>
       </c>
       <c r="B162" s="1">
-        <v>96.701183999999998</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -8731,7 +8731,7 @@
         <v>14</v>
       </c>
       <c r="B163" s="1">
-        <v>95.269751999999997</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -8739,7 +8739,7 @@
         <v>14</v>
       </c>
       <c r="B164" s="1">
-        <v>96.542135999999999</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -8747,7 +8747,7 @@
         <v>14</v>
       </c>
       <c r="B165" s="1">
-        <v>96.064992000000004</v>
+        <v>128.12824800000001</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -8755,7 +8755,7 @@
         <v>14</v>
       </c>
       <c r="B166" s="1">
-        <v>96.064992000000004</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -8763,7 +8763,7 @@
         <v>14</v>
       </c>
       <c r="B167" s="1">
-        <v>96.224039999999903</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -8771,7 +8771,7 @@
         <v>14</v>
       </c>
       <c r="B168" s="1">
-        <v>96.542135999999999</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -8779,7 +8779,7 @@
         <v>14</v>
       </c>
       <c r="B169" s="1">
-        <v>96.542135999999999</v>
+        <v>123.585804</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -8787,7 +8787,7 @@
         <v>14</v>
       </c>
       <c r="B170" s="1">
-        <v>96.224039999999903</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -8795,7 +8795,7 @@
         <v>14</v>
       </c>
       <c r="B171" s="1">
-        <v>96.383087999999901</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -8803,7 +8803,7 @@
         <v>14</v>
       </c>
       <c r="B172" s="1">
-        <v>96.064992000000004</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -8811,7 +8811,7 @@
         <v>14</v>
       </c>
       <c r="B173" s="1">
-        <v>96.064992000000004</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -8819,7 +8819,7 @@
         <v>14</v>
       </c>
       <c r="B174" s="1">
-        <v>97.019279999999995</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -8827,7 +8827,7 @@
         <v>14</v>
       </c>
       <c r="B175" s="1">
-        <v>96.701183999999998</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -8835,7 +8835,7 @@
         <v>14</v>
       </c>
       <c r="B176" s="1">
-        <v>98.132615999999999</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -8843,7 +8843,7 @@
         <v>14</v>
       </c>
       <c r="B177" s="1">
-        <v>96.224039999999903</v>
+        <v>127.031796</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -8851,7 +8851,7 @@
         <v>14</v>
       </c>
       <c r="B178" s="1">
-        <v>96.064992000000004</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -8859,7 +8859,7 @@
         <v>14</v>
       </c>
       <c r="B179" s="1">
-        <v>96.542135999999999</v>
+        <v>127.65834</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
@@ -8867,7 +8867,7 @@
         <v>14</v>
       </c>
       <c r="B180" s="1">
-        <v>97.973568</v>
+        <v>128.28488399999901</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -8875,7 +8875,7 @@
         <v>14</v>
       </c>
       <c r="B181" s="1">
-        <v>96.860231999999996</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -8883,7 +8883,7 @@
         <v>14</v>
       </c>
       <c r="B182" s="1">
-        <v>96.064992000000004</v>
+        <v>127.501704</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -8891,7 +8891,7 @@
         <v>14</v>
       </c>
       <c r="B183" s="1">
-        <v>96.383087999999901</v>
+        <v>127.188431999999</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -8899,7 +8899,7 @@
         <v>14</v>
       </c>
       <c r="B184" s="1">
-        <v>96.224039999999903</v>
+        <v>127.97161199999999</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -8907,7 +8907,7 @@
         <v>14</v>
       </c>
       <c r="B185" s="1">
-        <v>96.383087999999901</v>
+        <v>127.345068</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -8915,7 +8915,7 @@
         <v>14</v>
       </c>
       <c r="B186" s="1">
-        <v>97.178327999999993</v>
+        <v>124.838892</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -8923,7 +8923,7 @@
         <v>14</v>
       </c>
       <c r="B187" s="1">
-        <v>95.746895999999893</v>
+        <v>127.188431999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>